<commit_message>
Correccion del Spring 3
</commit_message>
<xml_diff>
--- a/SCRUM SPRINT 3 BACKLOG.xlsx
+++ b/SCRUM SPRINT 3 BACKLOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiencia profesional 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC0E360-08A5-4705-AB6A-0337F5CD981F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD531F35-B66B-4FCD-946D-8F4770A15128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8B89645F-FAD9-E44E-8B8A-333AB521BF6B}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="SCRUM SPRINT 2 BACKLOG" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Identificador (ID) de item de product backlog</t>
   </si>
@@ -59,37 +60,106 @@
     <t>Jahel Chacon</t>
   </si>
   <si>
-    <t>Muestra la localizacion</t>
-  </si>
-  <si>
-    <t>Creacion de la burbuja de aproximidad</t>
-  </si>
-  <si>
-    <t>Detalle de diseño</t>
-  </si>
-  <si>
-    <t>Implementacion de segunda cuenta</t>
-  </si>
-  <si>
-    <t>Muestra de segundo punto</t>
-  </si>
-  <si>
-    <t>Añadido de proximidad</t>
-  </si>
-  <si>
-    <t>Creacion de Scrum</t>
-  </si>
-  <si>
-    <t>Creacion de Diagrama</t>
-  </si>
-  <si>
-    <t>Creacion de Documeno final</t>
-  </si>
-  <si>
-    <t>Documentacion del codigo</t>
-  </si>
-  <si>
-    <t>Documentacion del proyecto</t>
+    <t>Insertar usuarios de ejemplo</t>
+  </si>
+  <si>
+    <t>Probar mapa de aplicación en Desktop y Mobile</t>
+  </si>
+  <si>
+    <t>Crear mapa con Google Maps</t>
+  </si>
+  <si>
+    <t>Integrar mapa con 2 botones, uno de coordenadas y otro de mostrar mapa</t>
+  </si>
+  <si>
+    <t>Crear e incluir script para mapa</t>
+  </si>
+  <si>
+    <t>Actualizar datos del usuario en el form</t>
+  </si>
+  <si>
+    <t>Obtener datos del usuario para form</t>
+  </si>
+  <si>
+    <t>Crear form básico con datos del usuario</t>
+  </si>
+  <si>
+    <t>Crear página de cuenta</t>
+  </si>
+  <si>
+    <t>Integrar Longitud y Latitud en el mapa para obtener localización actual </t>
+  </si>
+  <si>
+    <t>Investigar cómo notificar según la proximidad de las personas</t>
+  </si>
+  <si>
+    <t>Crear ejemplo funcional con notificación según localización por GPS</t>
+  </si>
+  <si>
+    <t>Investigar API de Google para crear rango circular a partir de la ubicación del usuario</t>
+  </si>
+  <si>
+    <t>Probar ejemplo funcional con notificación por GPS</t>
+  </si>
+  <si>
+    <t>Crear ejemplo funcional donde se cree un rango circular desde la ubicación del usuario</t>
+  </si>
+  <si>
+    <t>Investigar librería para realizar una acción dependiendo de si está dentro de un rango de localización</t>
+  </si>
+  <si>
+    <t>Integrar librería de acción dentro de rango de localización con previo ejemplo de creación de círculo según ubicación del usuario</t>
+  </si>
+  <si>
+    <t>Integrar ejemplo funcional por notificación por GPS dentro de la solución de la página web</t>
+  </si>
+  <si>
+    <t>Investigar sesiones en PHP</t>
+  </si>
+  <si>
+    <t>Probar que funcione correctamente la integración del ejemplo de notificación por GPS</t>
+  </si>
+  <si>
+    <t>Integrar combinación de funcionalidades donde el usuario pueda ver su ubicación, dibujar un rango circular alrededor suyo, y que realice una acción al estar cerca de otro usuario</t>
+  </si>
+  <si>
+    <t>Habilitar funcionalidad para saber cuando 1 o más usuarios estén conectados en la aplicación, al mismo tiempo que su ubicación actual.</t>
+  </si>
+  <si>
+    <t>Crear botón para guardar ubicación del usuario en base de datos</t>
+  </si>
+  <si>
+    <t>Mostar notificación si otro usuario está cerca y además está activo</t>
+  </si>
+  <si>
+    <t>Test de la aplicación</t>
+  </si>
+  <si>
+    <t>Implementacion de mapa</t>
+  </si>
+  <si>
+    <t>Informacion del usuario</t>
+  </si>
+  <si>
+    <t>Coordenadas de mapa</t>
+  </si>
+  <si>
+    <t>Investigaion de notificaciones del mapa</t>
+  </si>
+  <si>
+    <t>Rango de proximidad</t>
+  </si>
+  <si>
+    <t>Notificacion de proximidad</t>
+  </si>
+  <si>
+    <t>Sesion de usuario con PHP</t>
+  </si>
+  <si>
+    <t>Prueba de la aplicación</t>
+  </si>
+  <si>
+    <t>Funionalidades extra</t>
   </si>
 </sst>
 </file>
@@ -140,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -172,11 +242,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -186,6 +267,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF01BFD-5254-5340-9D06-B26DEBDD9471}">
-  <dimension ref="A3:E12"/>
+  <dimension ref="A3:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="A13:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -520,13 +604,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -545,12 +629,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -562,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -580,10 +664,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
@@ -605,15 +689,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
+    <row r="9" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
@@ -622,11 +702,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
@@ -639,7 +723,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>6</v>
@@ -652,19 +736,259 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="78" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>